<commit_message>
Rebulid done - NOT WORKING!
</commit_message>
<xml_diff>
--- a/Tabela_sil.xlsx
+++ b/Tabela_sil.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PWR RACING TEAM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8457dc860e8908b/Pwr Racing/RT_Vehicle_Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA6ED514-8467-4D4A-ADF2-858844FE3B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{FA6ED514-8467-4D4A-ADF2-858844FE3B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38075F28-0ECB-490E-8B01-69C74FB510C3}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{C25EDFAC-58AC-4739-91C9-5963E2B24EEA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C25EDFAC-58AC-4739-91C9-5963E2B24EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Fy" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -133,6 +130,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -156,9 +156,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -196,7 +196,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -302,7 +302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -444,7 +444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -458,270 +458,270 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>-20</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>-19.5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>-19</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>-18.5</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>-18</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>-17.5</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>-17</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>-16.5</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>-16</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>-15.5</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>-15</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>-14.5</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>-14</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>-13.5</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="1">
         <v>-13</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="1">
         <v>-12.5</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="1">
         <v>-12</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
         <v>-11.5</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="1">
         <v>-11</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="1">
         <v>-10.5</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="1">
         <v>-10</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="1">
         <v>-9.5</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="1">
         <v>-9</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="1">
         <v>-8.5</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="1">
         <v>-8</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="1">
         <v>-7.5</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2" s="1">
         <v>-7</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2" s="1">
         <v>-6.5</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AE2" s="1">
         <v>-6</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AF2" s="1">
         <v>-5.5</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AG2" s="1">
         <v>-5</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AH2" s="1">
         <v>-4.5</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AI2" s="1">
         <v>-4</v>
       </c>
-      <c r="AJ2" s="2">
+      <c r="AJ2" s="1">
         <v>-3.5</v>
       </c>
-      <c r="AK2" s="2">
+      <c r="AK2" s="1">
         <v>-3</v>
       </c>
-      <c r="AL2" s="2">
+      <c r="AL2" s="1">
         <v>-2.5</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="AM2" s="1">
         <v>-2</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AN2" s="1">
         <v>-1.5</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="AO2" s="1">
         <v>-1</v>
       </c>
-      <c r="AP2" s="2">
+      <c r="AP2" s="1">
         <v>-0.5</v>
       </c>
-      <c r="AQ2" s="2">
+      <c r="AQ2" s="1">
         <v>0</v>
       </c>
-      <c r="AR2" s="2">
+      <c r="AR2" s="1">
         <v>0.5</v>
       </c>
-      <c r="AS2" s="2">
+      <c r="AS2" s="1">
         <v>1</v>
       </c>
-      <c r="AT2" s="2">
+      <c r="AT2" s="1">
         <v>1.5</v>
       </c>
-      <c r="AU2" s="2">
+      <c r="AU2" s="1">
         <v>2</v>
       </c>
-      <c r="AV2" s="2">
+      <c r="AV2" s="1">
         <v>2.5</v>
       </c>
-      <c r="AW2" s="2">
+      <c r="AW2" s="1">
         <v>3</v>
       </c>
-      <c r="AX2" s="2">
+      <c r="AX2" s="1">
         <v>3.5</v>
       </c>
-      <c r="AY2" s="2">
+      <c r="AY2" s="1">
         <v>4</v>
       </c>
-      <c r="AZ2" s="2">
+      <c r="AZ2" s="1">
         <v>4.5</v>
       </c>
-      <c r="BA2" s="2">
+      <c r="BA2" s="1">
         <v>5</v>
       </c>
-      <c r="BB2" s="2">
+      <c r="BB2" s="1">
         <v>5.5</v>
       </c>
-      <c r="BC2" s="2">
+      <c r="BC2" s="1">
         <v>6</v>
       </c>
-      <c r="BD2" s="2">
+      <c r="BD2" s="1">
         <v>6.5</v>
       </c>
-      <c r="BE2" s="2">
+      <c r="BE2" s="1">
         <v>7</v>
       </c>
-      <c r="BF2" s="2">
+      <c r="BF2" s="1">
         <v>7.5</v>
       </c>
-      <c r="BG2" s="2">
+      <c r="BG2" s="1">
         <v>8</v>
       </c>
-      <c r="BH2" s="2">
+      <c r="BH2" s="1">
         <v>8.5</v>
       </c>
-      <c r="BI2" s="2">
+      <c r="BI2" s="1">
         <v>9</v>
       </c>
-      <c r="BJ2" s="2">
+      <c r="BJ2" s="1">
         <v>9.5</v>
       </c>
-      <c r="BK2" s="2">
+      <c r="BK2" s="1">
         <v>10</v>
       </c>
-      <c r="BL2" s="2">
+      <c r="BL2" s="1">
         <v>10.5</v>
       </c>
-      <c r="BM2" s="2">
+      <c r="BM2" s="1">
         <v>11</v>
       </c>
-      <c r="BN2" s="2">
+      <c r="BN2" s="1">
         <v>11.5</v>
       </c>
-      <c r="BO2" s="2">
+      <c r="BO2" s="1">
         <v>12</v>
       </c>
-      <c r="BP2" s="2">
+      <c r="BP2" s="1">
         <v>12.5</v>
       </c>
-      <c r="BQ2" s="2">
+      <c r="BQ2" s="1">
         <v>13</v>
       </c>
-      <c r="BR2" s="2">
+      <c r="BR2" s="1">
         <v>13.5</v>
       </c>
-      <c r="BS2" s="2">
+      <c r="BS2" s="1">
         <v>14</v>
       </c>
-      <c r="BT2" s="2">
+      <c r="BT2" s="1">
         <v>14.5</v>
       </c>
-      <c r="BU2" s="2">
+      <c r="BU2" s="1">
         <v>15</v>
       </c>
-      <c r="BV2" s="2">
+      <c r="BV2" s="1">
         <v>15.5</v>
       </c>
-      <c r="BW2" s="2">
+      <c r="BW2" s="1">
         <v>16</v>
       </c>
-      <c r="BX2" s="2">
+      <c r="BX2" s="1">
         <v>16.5</v>
       </c>
-      <c r="BY2" s="2">
+      <c r="BY2" s="1">
         <v>17</v>
       </c>
-      <c r="BZ2" s="2">
+      <c r="BZ2" s="1">
         <v>17.5</v>
       </c>
-      <c r="CA2" s="2">
+      <c r="CA2" s="1">
         <v>18</v>
       </c>
-      <c r="CB2" s="2">
+      <c r="CB2" s="1">
         <v>18.5</v>
       </c>
-      <c r="CC2" s="2">
+      <c r="CC2" s="1">
         <v>19</v>
       </c>
-      <c r="CD2" s="2">
+      <c r="CD2" s="1">
         <v>19.5</v>
       </c>
-      <c r="CE2" s="2">
+      <c r="CE2" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3">
@@ -968,8 +968,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B4" s="3">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
         <v>50</v>
       </c>
       <c r="C4">
@@ -1216,8 +1216,8 @@
         <v>-72.087045718056004</v>
       </c>
     </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B5" s="3">
+    <row r="5" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
         <v>100</v>
       </c>
       <c r="C5">
@@ -1464,8 +1464,8 @@
         <v>-143.57376897459699</v>
       </c>
     </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B6" s="3">
+    <row r="6" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
         <v>150</v>
       </c>
       <c r="C6">
@@ -1712,8 +1712,8 @@
         <v>-214.548035200843</v>
       </c>
     </row>
-    <row r="7" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B7" s="3">
+    <row r="7" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
         <v>200</v>
       </c>
       <c r="C7">
@@ -1960,8 +1960,8 @@
         <v>-285.09340514345701</v>
       </c>
     </row>
-    <row r="8" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B8" s="3">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
         <v>250</v>
       </c>
       <c r="C8">
@@ -2208,8 +2208,8 @@
         <v>-355.28874824951902</v>
       </c>
     </row>
-    <row r="9" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B9" s="3">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
         <v>300</v>
       </c>
       <c r="C9">
@@ -2456,8 +2456,8 @@
         <v>-425.20803611087098</v>
       </c>
     </row>
-    <row r="10" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B10" s="3">
+    <row r="10" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
         <v>350</v>
       </c>
       <c r="C10">
@@ -2704,8 +2704,8 @@
         <v>-494.92027602451799</v>
       </c>
     </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B11" s="3">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
         <v>400</v>
       </c>
       <c r="C11">
@@ -2952,8 +2952,8 @@
         <v>-564.48955091734103</v>
       </c>
     </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B12" s="3">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
         <v>450</v>
       </c>
       <c r="C12">
@@ -3200,8 +3200,8 @@
         <v>-633.97513757271099</v>
       </c>
     </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B13" s="3">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
         <v>500</v>
       </c>
       <c r="C13">
@@ -3448,8 +3448,8 @@
         <v>-703.43168017031701</v>
       </c>
     </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B14" s="3">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
         <v>550</v>
       </c>
       <c r="C14">
@@ -3696,8 +3696,8 @@
         <v>-772.90940057156797</v>
       </c>
     </row>
-    <row r="15" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B15" s="3">
+    <row r="15" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
         <v>600</v>
       </c>
       <c r="C15">
@@ -3944,8 +3944,8 @@
         <v>-842.45433056371098</v>
       </c>
     </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.45">
-      <c r="B16" s="3">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
         <v>650</v>
       </c>
       <c r="C16">
@@ -4192,8 +4192,8 @@
         <v>-912.10855445844697</v>
       </c>
     </row>
-    <row r="17" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B17" s="3">
+    <row r="17" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
         <v>700</v>
       </c>
       <c r="C17">
@@ -4440,8 +4440,8 @@
         <v>-981.91045308389596</v>
       </c>
     </row>
-    <row r="18" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B18" s="3">
+    <row r="18" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
         <v>750</v>
       </c>
       <c r="C18">
@@ -4688,8 +4688,8 @@
         <v>-1051.8949423771401</v>
       </c>
     </row>
-    <row r="19" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B19" s="3">
+    <row r="19" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
         <v>800</v>
       </c>
       <c r="C19">
@@ -4936,8 +4936,8 @@
         <v>-1122.0937015438101</v>
       </c>
     </row>
-    <row r="20" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B20" s="3">
+    <row r="20" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
         <v>850</v>
       </c>
       <c r="C20">
@@ -5184,8 +5184,8 @@
         <v>-1192.53538716358</v>
       </c>
     </row>
-    <row r="21" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B21" s="3">
+    <row r="21" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B21" s="2">
         <v>900</v>
       </c>
       <c r="C21">
@@ -5432,8 +5432,8 @@
         <v>-1263.2458307432601</v>
       </c>
     </row>
-    <row r="22" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B22" s="3">
+    <row r="22" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
         <v>950</v>
       </c>
       <c r="C22">
@@ -5680,8 +5680,8 @@
         <v>-1334.2482181021201</v>
       </c>
     </row>
-    <row r="23" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B23" s="3">
+    <row r="23" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
         <v>1000</v>
       </c>
       <c r="C23">
@@ -5928,8 +5928,8 @@
         <v>-1405.5632496631899</v>
       </c>
     </row>
-    <row r="24" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B24" s="3">
+    <row r="24" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
         <v>1050</v>
       </c>
       <c r="C24">
@@ -6176,8 +6176,8 @@
         <v>-1477.20928125467</v>
       </c>
     </row>
-    <row r="25" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B25" s="3">
+    <row r="25" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
         <v>1100</v>
       </c>
       <c r="C25">
@@ -6424,8 +6424,8 @@
         <v>-1549.20244543238</v>
       </c>
     </row>
-    <row r="26" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B26" s="3">
+    <row r="26" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B26" s="2">
         <v>1150</v>
       </c>
       <c r="C26">
@@ -6672,8 +6672,8 @@
         <v>-1621.5567536410399</v>
       </c>
     </row>
-    <row r="27" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B27" s="3">
+    <row r="27" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
         <v>1200</v>
       </c>
       <c r="C27">
@@ -6920,8 +6920,8 @@
         <v>-1694.2841797639401</v>
       </c>
     </row>
-    <row r="28" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B28" s="3">
+    <row r="28" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
         <v>1250</v>
       </c>
       <c r="C28">
@@ -7168,8 +7168,8 @@
         <v>-1767.3947257833199</v>
       </c>
     </row>
-    <row r="29" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B29" s="3">
+    <row r="29" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
         <v>1300</v>
       </c>
       <c r="C29">
@@ -7416,8 +7416,8 @@
         <v>-1840.896470404</v>
       </c>
     </row>
-    <row r="30" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B30" s="3">
+    <row r="30" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
         <v>1350</v>
       </c>
       <c r="C30">
@@ -7664,8 +7664,8 @@
         <v>-1914.7956015908201</v>
       </c>
     </row>
-    <row r="31" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B31" s="3">
+    <row r="31" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
         <v>1400</v>
       </c>
       <c r="C31">
@@ -7912,8 +7912,8 @@
         <v>-1989.0964340473799</v>
       </c>
     </row>
-    <row r="32" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B32" s="3">
+    <row r="32" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
         <v>1450</v>
       </c>
       <c r="C32">
@@ -8160,8 +8160,8 @@
         <v>-2063.8014127254701</v>
       </c>
     </row>
-    <row r="33" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B33" s="3">
+    <row r="33" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B33" s="2">
         <v>1500</v>
       </c>
       <c r="C33">
@@ -8408,8 +8408,8 @@
         <v>-2138.9111035083401</v>
       </c>
     </row>
-    <row r="34" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B34" s="3">
+    <row r="34" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
         <v>1550</v>
       </c>
       <c r="C34">
@@ -8656,8 +8656,8 @@
         <v>-2214.4241722602101</v>
       </c>
     </row>
-    <row r="35" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B35" s="3">
+    <row r="35" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B35" s="2">
         <v>1600</v>
       </c>
       <c r="C35">
@@ -8904,8 +8904,8 @@
         <v>-2290.3373534825701</v>
       </c>
     </row>
-    <row r="36" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B36" s="3">
+    <row r="36" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B36" s="2">
         <v>1650</v>
       </c>
       <c r="C36">
@@ -9152,8 +9152,8 @@
         <v>-2366.6454098673398</v>
       </c>
     </row>
-    <row r="37" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B37" s="3">
+    <row r="37" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B37" s="2">
         <v>1700</v>
       </c>
       <c r="C37">
@@ -9400,8 +9400,8 @@
         <v>-2443.3410840883398</v>
       </c>
     </row>
-    <row r="38" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B38" s="3">
+    <row r="38" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B38" s="2">
         <v>1750</v>
       </c>
       <c r="C38">
@@ -9648,8 +9648,8 @@
         <v>-2520.4150442272098</v>
       </c>
     </row>
-    <row r="39" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B39" s="3">
+    <row r="39" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B39" s="2">
         <v>1800</v>
       </c>
       <c r="C39">
@@ -9896,8 +9896,8 @@
         <v>-2597.8558242868698</v>
       </c>
     </row>
-    <row r="40" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B40" s="3">
+    <row r="40" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
         <v>1850</v>
       </c>
       <c r="C40">
@@ -10144,8 +10144,8 @@
         <v>-2675.64976130475</v>
       </c>
     </row>
-    <row r="41" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B41" s="3">
+    <row r="41" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
         <v>1900</v>
       </c>
       <c r="C41">
@@ -10392,8 +10392,8 @@
         <v>-2753.7809306377699</v>
       </c>
     </row>
-    <row r="42" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B42" s="3">
+    <row r="42" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
         <v>1950</v>
       </c>
       <c r="C42">
@@ -10640,8 +10640,8 @@
         <v>-2832.2310810497402</v>
       </c>
     </row>
-    <row r="43" spans="2:83" x14ac:dyDescent="0.45">
-      <c r="B43" s="3">
+    <row r="43" spans="2:83" x14ac:dyDescent="0.3">
+      <c r="B43" s="2">
         <v>2000</v>
       </c>
       <c r="C43">
@@ -10900,20 +10900,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF4287F-AFFE-4396-9055-1B1355798A33}">
   <dimension ref="A1:AQ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AR31" sqref="AR31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
@@ -10927,139 +10927,139 @@
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>-0.2</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>-0.19</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>-0.18</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>-0.17</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>-0.16</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>-0.15</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>-0.13</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>-0.12</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>-0.11</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>-0.1</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>-0.09</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <v>-0.08</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="5">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="5">
         <v>-0.06</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="5">
         <v>-0.05</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="5">
         <v>-0.04</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="5">
         <v>-0.03</v>
       </c>
-      <c r="U4" s="6">
+      <c r="U4" s="5">
         <v>-0.02</v>
       </c>
-      <c r="V4" s="6">
+      <c r="V4" s="5">
         <v>-0.01</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="5">
         <v>0</v>
       </c>
-      <c r="X4" s="6">
+      <c r="X4" s="5">
         <v>9.9999999999999794E-3</v>
       </c>
-      <c r="Y4" s="6">
+      <c r="Y4" s="5">
         <v>0.02</v>
       </c>
-      <c r="Z4" s="6">
+      <c r="Z4" s="5">
         <v>0.03</v>
       </c>
-      <c r="AA4" s="6">
+      <c r="AA4" s="5">
         <v>0.04</v>
       </c>
-      <c r="AB4" s="6">
+      <c r="AB4" s="5">
         <v>0.05</v>
       </c>
-      <c r="AC4" s="6">
+      <c r="AC4" s="5">
         <v>0.06</v>
       </c>
-      <c r="AD4" s="6">
+      <c r="AD4" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="AE4" s="6">
+      <c r="AE4" s="5">
         <v>0.08</v>
       </c>
-      <c r="AF4" s="6">
+      <c r="AF4" s="5">
         <v>0.09</v>
       </c>
-      <c r="AG4" s="6">
+      <c r="AG4" s="5">
         <v>0.1</v>
       </c>
-      <c r="AH4" s="6">
+      <c r="AH4" s="5">
         <v>0.11</v>
       </c>
-      <c r="AI4" s="6">
+      <c r="AI4" s="5">
         <v>0.12</v>
       </c>
-      <c r="AJ4" s="6">
+      <c r="AJ4" s="5">
         <v>0.13</v>
       </c>
-      <c r="AK4" s="6">
+      <c r="AK4" s="5">
         <v>0.14000000000000001</v>
       </c>
-      <c r="AL4" s="6">
+      <c r="AL4" s="5">
         <v>0.15</v>
       </c>
-      <c r="AM4" s="6">
+      <c r="AM4" s="5">
         <v>0.16</v>
       </c>
-      <c r="AN4" s="6">
+      <c r="AN4" s="5">
         <v>0.17</v>
       </c>
-      <c r="AO4" s="6">
+      <c r="AO4" s="5">
         <v>0.18</v>
       </c>
-      <c r="AP4" s="6">
+      <c r="AP4" s="5">
         <v>0.19</v>
       </c>
-      <c r="AQ4" s="6">
+      <c r="AQ4" s="5">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>0</v>
       </c>
       <c r="C5">
@@ -11186,8 +11186,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B6" s="3">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
         <v>50</v>
       </c>
       <c r="C6">
@@ -11314,8 +11314,8 @@
         <v>-70.033972749569102</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B7" s="3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
         <v>100</v>
       </c>
       <c r="C7">
@@ -11442,8 +11442,8 @@
         <v>-135.61486614009499</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B8" s="3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
         <v>150</v>
       </c>
       <c r="C8">
@@ -11570,8 +11570,8 @@
         <v>-194.36552900402501</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B9" s="3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
         <v>200</v>
       </c>
       <c r="C9">
@@ -11698,8 +11698,8 @@
         <v>-242.59403604426501</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B10" s="3">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
         <v>250</v>
       </c>
       <c r="C10">
@@ -11826,8 +11826,8 @@
         <v>-274.68792723520301</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B11" s="3">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
         <v>300</v>
       </c>
       <c r="C11">
@@ -11954,8 +11954,8 @@
         <v>-282.48778025037001</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B12" s="3">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
         <v>350</v>
       </c>
       <c r="C12">
@@ -12082,8 +12082,8 @@
         <v>-255.145016480706</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B13" s="3">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
         <v>400</v>
       </c>
       <c r="C13">
@@ -12210,8 +12210,8 @@
         <v>-180.638904951336</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B14" s="3">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B14" s="2">
         <v>450</v>
       </c>
       <c r="C14">
@@ -12338,8 +12338,8 @@
         <v>-50.485687297480702</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B15" s="3">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
         <v>500</v>
       </c>
       <c r="C15">
@@ -12466,8 +12466,8 @@
         <v>132.806258675707</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.45">
-      <c r="B16" s="3">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
         <v>550</v>
       </c>
       <c r="C16">
@@ -12594,8 +12594,8 @@
         <v>351.24498144229398</v>
       </c>
     </row>
-    <row r="17" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B17" s="3">
+    <row r="17" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
         <v>600</v>
       </c>
       <c r="C17">
@@ -12722,8 +12722,8 @@
         <v>577.073170898787</v>
       </c>
     </row>
-    <row r="18" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B18" s="3">
+    <row r="18" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
         <v>650</v>
       </c>
       <c r="C18">
@@ -12850,8 +12850,8 @@
         <v>785.79119424835801</v>
       </c>
     </row>
-    <row r="19" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B19" s="3">
+    <row r="19" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
         <v>700</v>
       </c>
       <c r="C19">
@@ -12978,8 +12978,8 @@
         <v>964.65081984114897</v>
       </c>
     </row>
-    <row r="20" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B20" s="3">
+    <row r="20" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
         <v>750</v>
       </c>
       <c r="C20">
@@ -13106,8 +13106,8 @@
         <v>1111.8346230085599</v>
       </c>
     </row>
-    <row r="21" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B21" s="3">
+    <row r="21" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B21" s="2">
         <v>800</v>
       </c>
       <c r="C21">
@@ -13234,8 +13234,8 @@
         <v>1231.3649744847801</v>
       </c>
     </row>
-    <row r="22" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B22" s="3">
+    <row r="22" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
         <v>850</v>
       </c>
       <c r="C22">
@@ -13362,8 +13362,8 @@
         <v>1328.8900259193799</v>
       </c>
     </row>
-    <row r="23" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B23" s="3">
+    <row r="23" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
         <v>900</v>
       </c>
       <c r="C23">
@@ -13490,8 +13490,8 @@
         <v>1409.60461255631</v>
       </c>
     </row>
-    <row r="24" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B24" s="3">
+    <row r="24" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
         <v>950</v>
       </c>
       <c r="C24">
@@ -13618,8 +13618,8 @@
         <v>1477.6185559564501</v>
       </c>
     </row>
-    <row r="25" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B25" s="3">
+    <row r="25" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
         <v>1000</v>
       </c>
       <c r="C25">
@@ -13746,8 +13746,8 @@
         <v>1535.9711791171301</v>
       </c>
     </row>
-    <row r="26" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B26" s="3">
+    <row r="26" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B26" s="2">
         <v>1050</v>
       </c>
       <c r="C26">
@@ -13874,8 +13874,8 @@
         <v>1586.8429637255699</v>
       </c>
     </row>
-    <row r="27" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B27" s="3">
+    <row r="27" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
         <v>1100</v>
       </c>
       <c r="C27">
@@ -14002,8 +14002,8 @@
         <v>1631.7806420013501</v>
       </c>
     </row>
-    <row r="28" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B28" s="3">
+    <row r="28" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
         <v>1150</v>
       </c>
       <c r="C28">
@@ -14130,8 +14130,8 @@
         <v>1671.8804294383301</v>
       </c>
     </row>
-    <row r="29" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B29" s="3">
+    <row r="29" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
         <v>1200</v>
       </c>
       <c r="C29">
@@ -14258,8 +14258,8 @@
         <v>1707.9232564587401</v>
       </c>
     </row>
-    <row r="30" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B30" s="3">
+    <row r="30" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
         <v>1250</v>
       </c>
       <c r="C30">
@@ -14386,8 +14386,8 @@
         <v>1740.4704460871101</v>
       </c>
     </row>
-    <row r="31" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B31" s="3">
+    <row r="31" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
         <v>1300</v>
       </c>
       <c r="C31">
@@ -14514,8 +14514,8 @@
         <v>1769.93025887369</v>
       </c>
     </row>
-    <row r="32" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B32" s="3">
+    <row r="32" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
         <v>1350</v>
       </c>
       <c r="C32">
@@ -14642,8 +14642,8 @@
         <v>1796.60399782228</v>
       </c>
     </row>
-    <row r="33" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B33" s="3">
+    <row r="33" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B33" s="2">
         <v>1400</v>
       </c>
       <c r="C33">
@@ -14770,8 +14770,8 @@
         <v>1820.71808312844</v>
       </c>
     </row>
-    <row r="34" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B34" s="3">
+    <row r="34" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
         <v>1450</v>
       </c>
       <c r="C34">
@@ -14898,8 +14898,8 @@
         <v>1842.44658651847</v>
       </c>
     </row>
-    <row r="35" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B35" s="3">
+    <row r="35" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B35" s="2">
         <v>1500</v>
       </c>
       <c r="C35">
@@ -15026,8 +15026,8 @@
         <v>1861.9273048980599</v>
       </c>
     </row>
-    <row r="36" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B36" s="3">
+    <row r="36" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B36" s="2">
         <v>1550</v>
       </c>
       <c r="C36">
@@ -15154,8 +15154,8 @@
         <v>1879.27347670312</v>
       </c>
     </row>
-    <row r="37" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B37" s="3">
+    <row r="37" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B37" s="2">
         <v>1600</v>
       </c>
       <c r="C37">
@@ -15282,8 +15282,8 @@
         <v>1894.5825887345</v>
       </c>
     </row>
-    <row r="38" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B38" s="3">
+    <row r="38" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B38" s="2">
         <v>1650</v>
       </c>
       <c r="C38">
@@ -15410,8 +15410,8 @@
         <v>1907.9432903424699</v>
       </c>
     </row>
-    <row r="39" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B39" s="3">
+    <row r="39" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B39" s="2">
         <v>1700</v>
       </c>
       <c r="C39">
@@ -15538,8 +15538,8 @@
         <v>1919.44115603514</v>
       </c>
     </row>
-    <row r="40" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B40" s="3">
+    <row r="40" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
         <v>1750</v>
       </c>
       <c r="C40">
@@ -15666,8 +15666,8 @@
         <v>1929.1638703435301</v>
       </c>
     </row>
-    <row r="41" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B41" s="3">
+    <row r="41" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
         <v>1800</v>
       </c>
       <c r="C41">
@@ -15794,8 +15794,8 @@
         <v>1937.2063208058501</v>
       </c>
     </row>
-    <row r="42" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B42" s="3">
+    <row r="42" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
         <v>1850</v>
       </c>
       <c r="C42">
@@ -15922,8 +15922,8 @@
         <v>1943.6760591253999</v>
       </c>
     </row>
-    <row r="43" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B43" s="3">
+    <row r="43" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B43" s="2">
         <v>1900</v>
       </c>
       <c r="C43">
@@ -16050,8 +16050,8 @@
         <v>1948.69961731278</v>
       </c>
     </row>
-    <row r="44" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B44" s="3">
+    <row r="44" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
         <v>1950</v>
       </c>
       <c r="C44">
@@ -16178,8 +16178,8 @@
         <v>1952.4302364753601</v>
       </c>
     </row>
-    <row r="45" spans="2:43" x14ac:dyDescent="0.45">
-      <c r="B45" s="3">
+    <row r="45" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B45" s="2">
         <v>2000</v>
       </c>
       <c r="C45">
@@ -16311,6 +16311,18 @@
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="I1:R1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C6:AQ45">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>